<commit_message>
added data bevore picco
</commit_message>
<xml_diff>
--- a/20240321circuiti2/circuiti_2_dati.xlsx
+++ b/20240321circuiti2/circuiti_2_dati.xlsx
@@ -127,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
@@ -142,14 +142,17 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
-      <protection hidden="0" locked="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
-      <protection hidden="0" locked="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2902,7 +2905,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2912,7 +2915,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2927,7 +2930,7 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -2959,8 +2962,8 @@
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="10">
-        <v>7.4800000000000004</v>
+      <c r="F2" s="8">
+        <v>0</v>
       </c>
       <c r="G2" s="4">
         <v>8</v>
@@ -2972,666 +2975,825 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="E3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11">
+        <v>4</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11">
+        <v>12</v>
+      </c>
+      <c r="F5" s="8">
+        <v>5.7199999999999998</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8">
+        <v>6.4800000000000004</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8">
+        <v>6.9199999999999999</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11">
+        <v>24</v>
+      </c>
+      <c r="F8" s="8">
+        <v>7.2000000000000002</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11">
+        <v>28</v>
+      </c>
+      <c r="F9" s="8">
+        <v>7.3600000000000003</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11">
+        <v>32</v>
+      </c>
+      <c r="F10" s="8">
+        <v>7.4400000000000004</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11">
+        <v>36</v>
+      </c>
+      <c r="F11" s="8">
+        <v>7.4800000000000004</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>7.4800000000000004</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="E13" s="7">
         <v>40</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F13" s="2">
         <v>7.2400000000000002</v>
       </c>
     </row>
-    <row r="4" ht="14.25">
-      <c r="E4">
+    <row r="14" ht="14.25">
+      <c r="E14" s="7">
         <v>80</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F14" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="E5">
+    <row r="15" ht="14.25">
+      <c r="E15" s="7">
         <v>120</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F15" s="2">
         <v>6.7199999999999998</v>
       </c>
     </row>
-    <row r="6" ht="14.25">
-      <c r="E6" s="7">
+    <row r="16" ht="14.25">
+      <c r="E16" s="7">
         <v>160</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F16" s="2">
         <v>6.4800000000000004</v>
       </c>
     </row>
-    <row r="7" ht="14.25">
-      <c r="E7">
+    <row r="17" ht="14.25">
+      <c r="E17" s="7">
         <v>200</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F17" s="2">
         <v>6.2999999999999998</v>
       </c>
     </row>
-    <row r="8" ht="14.25">
-      <c r="E8">
+    <row r="18" ht="14.25">
+      <c r="E18" s="7">
         <v>240</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F18" s="2">
         <v>5.96</v>
       </c>
     </row>
-    <row r="9" ht="14.25">
-      <c r="E9">
+    <row r="19" ht="14.25">
+      <c r="E19" s="7">
         <v>280</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F19" s="2">
         <v>5.7599999999999998</v>
       </c>
     </row>
-    <row r="10" ht="14.25">
-      <c r="E10">
+    <row r="20" ht="14.25">
+      <c r="E20" s="7">
         <v>320</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F20" s="2">
         <v>5.5199999999999996</v>
       </c>
     </row>
-    <row r="11" ht="14.25">
-      <c r="E11">
+    <row r="21" ht="14.25">
+      <c r="E21" s="7">
         <v>360</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F21" s="2">
         <v>5.3200000000000003</v>
       </c>
     </row>
-    <row r="12" ht="14.25">
-      <c r="E12">
+    <row r="22" ht="14.25">
+      <c r="E22" s="7">
         <v>400</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F22" s="2">
         <v>5.0800000000000001</v>
       </c>
     </row>
-    <row r="13" ht="14.25">
-      <c r="E13">
+    <row r="23" ht="14.25">
+      <c r="E23" s="7">
         <v>440</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F23" s="2">
         <v>4.8799999999999999</v>
       </c>
     </row>
-    <row r="14" ht="14.25">
-      <c r="E14">
+    <row r="24" ht="14.25">
+      <c r="E24" s="7">
         <v>480</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F24" s="2">
         <v>4.6799999999999997</v>
       </c>
     </row>
-    <row r="15" ht="14.25">
-      <c r="E15">
+    <row r="25" ht="14.25">
+      <c r="E25" s="7">
         <v>520</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F25" s="2">
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="16" ht="14.25">
-      <c r="E16">
+    <row r="26" ht="14.25">
+      <c r="E26" s="7">
         <v>560</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F26" s="2">
         <v>4.3200000000000003</v>
       </c>
     </row>
-    <row r="17" ht="14.25">
-      <c r="E17">
+    <row r="27" ht="14.25">
+      <c r="E27" s="7">
         <v>600</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F27" s="2">
         <v>4.1600000000000001</v>
       </c>
     </row>
-    <row r="18" ht="14.25">
-      <c r="E18">
+    <row r="28" ht="14.25">
+      <c r="E28" s="7">
         <v>640</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F28" s="2">
         <v>3.96</v>
       </c>
     </row>
-    <row r="19" ht="14.25">
-      <c r="E19">
+    <row r="29" ht="14.25">
+      <c r="E29" s="7">
         <v>680</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F29" s="2">
         <v>3.8399999999999999</v>
       </c>
     </row>
-    <row r="20" ht="14.25">
-      <c r="E20">
+    <row r="30" ht="14.25">
+      <c r="E30" s="7">
         <v>720</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F30" s="2">
         <v>3.6400000000000001</v>
       </c>
     </row>
-    <row r="21" ht="14.25">
-      <c r="E21">
+    <row r="31" ht="14.25">
+      <c r="E31" s="7">
         <v>760</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F31" s="2">
         <v>3.52</v>
       </c>
     </row>
-    <row r="22" ht="14.25">
-      <c r="E22">
+    <row r="32" ht="14.25">
+      <c r="E32" s="7">
         <v>800</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F32" s="2">
         <v>3.3599999999999999</v>
       </c>
     </row>
-    <row r="23" ht="14.25">
-      <c r="E23">
+    <row r="33" ht="14.25">
+      <c r="E33" s="7">
         <v>840</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F33" s="2">
         <v>3.2400000000000002</v>
       </c>
     </row>
-    <row r="24" ht="14.25">
-      <c r="E24">
+    <row r="34" ht="14.25">
+      <c r="E34" s="7">
         <v>880</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F34" s="2">
         <v>3.0800000000000001</v>
       </c>
     </row>
-    <row r="25" ht="14.25">
-      <c r="E25">
+    <row r="35" ht="14.25">
+      <c r="E35" s="7">
         <v>920</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F35" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="26" ht="14.25">
-      <c r="E26">
+    <row r="36" ht="14.25">
+      <c r="E36" s="7">
         <v>960</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F36" s="2">
         <v>2.8799999999999999</v>
       </c>
     </row>
-    <row r="27" ht="14.25">
-      <c r="E27">
+    <row r="37" ht="14.25">
+      <c r="E37" s="7">
         <v>1000</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F37" s="2">
         <v>2.7599999999999998</v>
       </c>
     </row>
-    <row r="28" ht="14.25">
-      <c r="E28">
+    <row r="38" ht="14.25">
+      <c r="E38" s="7">
         <v>1040</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F38" s="2">
         <v>2.6400000000000001</v>
       </c>
     </row>
-    <row r="29" ht="14.25">
-      <c r="E29">
+    <row r="39" ht="14.25">
+      <c r="E39" s="7">
         <v>1080</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F39" s="2">
         <v>2.52</v>
       </c>
     </row>
-    <row r="30" ht="14.25">
-      <c r="E30">
+    <row r="40" ht="14.25">
+      <c r="E40" s="7">
         <v>1120</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F40" s="2">
         <v>2.4399999999999999</v>
       </c>
     </row>
-    <row r="31" ht="14.25">
-      <c r="E31">
+    <row r="41" ht="14.25">
+      <c r="E41" s="7">
         <v>1160</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F41" s="2">
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="32" ht="14.25">
-      <c r="E32">
+    <row r="42" ht="14.25">
+      <c r="E42" s="7">
         <v>1200</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F42" s="2">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="33" ht="14.25">
-      <c r="E33">
+    <row r="43" ht="14.25">
+      <c r="E43" s="7">
         <v>1240</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F43" s="2">
         <v>2.1200000000000001</v>
       </c>
     </row>
-    <row r="34" ht="14.25">
-      <c r="E34">
+    <row r="44" ht="14.25">
+      <c r="E44" s="7">
         <v>1280</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F44" s="2">
         <v>2.04</v>
       </c>
     </row>
-    <row r="35" ht="14.25">
-      <c r="E35">
+    <row r="45" ht="14.25">
+      <c r="E45" s="7">
         <v>1320</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F45" s="2">
         <v>1.96</v>
       </c>
     </row>
-    <row r="36" ht="14.25">
-      <c r="E36">
+    <row r="46" ht="14.25">
+      <c r="E46" s="7">
         <v>1360</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F46" s="2">
         <v>1.8799999999999999</v>
       </c>
     </row>
-    <row r="37" ht="14.25">
-      <c r="E37">
+    <row r="47" ht="14.25">
+      <c r="E47" s="7">
         <v>1400</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F47" s="2">
         <v>1.8</v>
       </c>
     </row>
-    <row r="38" ht="14.25">
-      <c r="E38">
+    <row r="48" ht="14.25">
+      <c r="E48" s="7">
         <v>1440</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F48" s="2">
         <v>1.76</v>
       </c>
     </row>
-    <row r="39" ht="14.25">
-      <c r="E39">
+    <row r="49" ht="14.25">
+      <c r="E49" s="7">
         <v>1480</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F49" s="2">
         <v>1.6799999999999999</v>
       </c>
     </row>
-    <row r="40" ht="14.25">
-      <c r="E40">
+    <row r="50" ht="14.25">
+      <c r="E50" s="7">
         <v>1520</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F50" s="2">
         <v>1.6000000000000001</v>
       </c>
     </row>
-    <row r="41" ht="14.25">
-      <c r="E41">
+    <row r="51" ht="14.25">
+      <c r="E51" s="7">
         <v>1560</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F51" s="2">
         <v>1.5600000000000001</v>
       </c>
     </row>
-    <row r="42" ht="14.25">
-      <c r="E42">
+    <row r="52" ht="14.25">
+      <c r="E52" s="7">
         <v>1600</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F52" s="2">
         <v>1.48</v>
       </c>
     </row>
-    <row r="43" ht="14.25">
-      <c r="E43">
+    <row r="53" ht="14.25">
+      <c r="E53" s="7">
         <v>1640</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F53" s="2">
         <v>1.4399999999999999</v>
       </c>
     </row>
-    <row r="44" ht="14.25">
-      <c r="E44">
+    <row r="54" ht="14.25">
+      <c r="E54" s="7">
         <v>1680</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F54" s="2">
         <v>1.3600000000000001</v>
       </c>
     </row>
-    <row r="45" ht="14.25">
-      <c r="E45">
+    <row r="55" ht="14.25">
+      <c r="E55" s="7">
         <v>1720</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F55" s="2">
         <v>1.3200000000000001</v>
       </c>
     </row>
-    <row r="46" ht="14.25">
-      <c r="E46">
+    <row r="56" ht="14.25">
+      <c r="E56" s="7">
         <v>1760</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F56" s="2">
         <v>1.28</v>
       </c>
     </row>
-    <row r="47" ht="14.25">
-      <c r="E47">
+    <row r="57" ht="14.25">
+      <c r="E57" s="7">
         <v>1800</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F57" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="48" ht="14.25">
-      <c r="E48">
+    <row r="58" ht="14.25">
+      <c r="E58" s="7">
         <v>1840</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F58" s="2">
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="49" ht="14.25">
-      <c r="E49">
+    <row r="59" ht="14.25">
+      <c r="E59" s="7">
         <v>1880</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F59" s="2">
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="50" ht="14.25">
-      <c r="E50">
+    <row r="60" ht="14.25">
+      <c r="E60" s="7">
         <v>1920</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F60" s="2">
         <v>1.0800000000000001</v>
       </c>
     </row>
-    <row r="51" ht="14.25">
-      <c r="E51">
+    <row r="61" ht="14.25">
+      <c r="E61" s="7">
         <v>1960</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F61" s="2">
         <v>1.04</v>
       </c>
     </row>
-    <row r="52" ht="14.25">
-      <c r="E52">
+    <row r="62" ht="14.25">
+      <c r="E62" s="7">
         <v>2000</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F62" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="53" ht="14.25">
-      <c r="E53">
+    <row r="63" ht="14.25">
+      <c r="E63" s="7">
         <v>2080</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F63" s="2">
         <v>0.92000000000000004</v>
       </c>
     </row>
-    <row r="54" ht="14.25">
-      <c r="E54">
+    <row r="64" ht="14.25">
+      <c r="E64" s="7">
         <v>2160</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F64" s="2">
         <v>0.83999999999999997</v>
       </c>
     </row>
-    <row r="55" ht="14.25">
-      <c r="E55">
+    <row r="65" ht="14.25">
+      <c r="E65" s="7">
         <v>2240</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F65" s="2">
         <v>0.76000000000000001</v>
       </c>
     </row>
-    <row r="56" ht="14.25">
-      <c r="E56">
+    <row r="66" ht="14.25">
+      <c r="E66" s="7">
         <v>2320</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F66" s="2">
         <v>0.71999999999999997</v>
       </c>
     </row>
-    <row r="57" ht="14.25">
-      <c r="E57">
+    <row r="67" ht="14.25">
+      <c r="E67" s="7">
         <v>2400</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F67" s="2">
         <v>0.64000000000000001</v>
       </c>
     </row>
-    <row r="58" ht="14.25">
-      <c r="E58">
+    <row r="68" ht="14.25">
+      <c r="E68" s="7">
         <v>2480</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F68" s="2">
         <v>0.59999999999999998</v>
       </c>
     </row>
-    <row r="59" ht="14.25">
-      <c r="E59">
+    <row r="69" ht="14.25">
+      <c r="E69" s="7">
         <v>2560</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F69" s="2">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="60" ht="14.25">
-      <c r="E60">
+    <row r="70" ht="14.25">
+      <c r="E70" s="7">
         <v>2640</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F70" s="2">
         <v>0.52000000000000002</v>
       </c>
     </row>
-    <row r="61" ht="14.25">
-      <c r="E61">
+    <row r="71" ht="14.25">
+      <c r="E71" s="7">
         <v>2720</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F71" s="2">
         <v>0.47999999999999998</v>
       </c>
     </row>
-    <row r="62" ht="14.25">
-      <c r="E62">
+    <row r="72" ht="14.25">
+      <c r="E72" s="7">
         <v>2800</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F72" s="2">
         <v>0.44</v>
       </c>
     </row>
-    <row r="63" ht="14.25">
-      <c r="E63">
+    <row r="73" ht="14.25">
+      <c r="E73" s="7">
         <v>2880</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F73" s="2">
         <v>0.40000000000000002</v>
       </c>
     </row>
-    <row r="64" ht="14.25">
-      <c r="E64">
+    <row r="74" ht="14.25">
+      <c r="E74" s="7">
         <v>2960</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F74" s="2">
         <v>0.40000000000000002</v>
       </c>
     </row>
-    <row r="65" ht="14.25">
-      <c r="E65">
+    <row r="75" ht="14.25">
+      <c r="E75" s="7">
         <v>3040</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F75" s="2">
         <v>0.35999999999999999</v>
       </c>
     </row>
-    <row r="66" ht="14.25">
-      <c r="E66">
+    <row r="76" ht="14.25">
+      <c r="E76" s="7">
         <v>3120</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F76" s="2">
         <v>0.32000000000000001</v>
       </c>
     </row>
-    <row r="67" ht="14.25">
-      <c r="E67">
+    <row r="77" ht="14.25">
+      <c r="E77" s="7">
         <v>3200</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F77" s="2">
         <v>0.32000000000000001</v>
       </c>
     </row>
-    <row r="68" ht="14.25">
-      <c r="E68">
+    <row r="78" ht="14.25">
+      <c r="E78" s="7">
         <v>3280</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F78" s="2">
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="69" ht="14.25">
-      <c r="E69">
+    <row r="79" ht="14.25">
+      <c r="E79" s="7">
         <v>3400</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F79" s="2">
         <v>0.23999999999999999</v>
       </c>
     </row>
-    <row r="70" ht="14.25">
-      <c r="E70">
+    <row r="80" ht="14.25">
+      <c r="E80" s="7">
         <v>3520</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F80" s="2">
         <v>0.20000000000000001</v>
       </c>
     </row>
-    <row r="71" ht="14.25">
-      <c r="E71">
+    <row r="81" ht="14.25">
+      <c r="E81" s="7">
         <v>3680</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F81" s="2">
         <v>0.20000000000000001</v>
       </c>
     </row>
-    <row r="72" ht="14.25">
-      <c r="E72">
+    <row r="82" ht="14.25">
+      <c r="E82" s="7">
         <v>3840</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F82" s="2">
         <v>0.16</v>
       </c>
     </row>
-    <row r="73" ht="14.25">
-      <c r="E73">
+    <row r="83" ht="14.25">
+      <c r="E83" s="7">
         <v>3920</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F83" s="2">
         <v>0.16</v>
       </c>
     </row>
-    <row r="74" ht="14.25">
-      <c r="E74">
+    <row r="84" ht="14.25">
+      <c r="E84" s="7">
         <v>4120</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F84" s="2">
         <v>0.12</v>
       </c>
     </row>
-    <row r="75" ht="14.25">
-      <c r="E75">
+    <row r="85" ht="14.25">
+      <c r="E85" s="7">
         <v>4320</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F85" s="2">
         <v>0.12</v>
       </c>
     </row>
-    <row r="76" ht="14.25">
-      <c r="E76">
+    <row r="86" ht="14.25">
+      <c r="E86" s="7">
         <v>4520</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F86" s="2">
         <v>0.080000000000000002</v>
       </c>
     </row>
-    <row r="77" ht="14.25">
-      <c r="E77">
+    <row r="87" ht="14.25">
+      <c r="E87" s="7">
         <v>4640</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F87" s="2">
         <v>0.080000000000000002</v>
       </c>
     </row>
-    <row r="78" ht="14.25">
-      <c r="E78">
+    <row r="88" ht="14.25">
+      <c r="E88" s="7">
         <v>4760</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F88" s="2">
         <v>0.080000000000000002</v>
       </c>
     </row>
-    <row r="79" ht="14.25">
-      <c r="E79">
+    <row r="89" ht="14.25">
+      <c r="E89" s="7">
         <v>5080</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F89" s="2">
         <v>0.040000000000000001</v>
       </c>
     </row>
-    <row r="80" ht="14.25">
-      <c r="E80">
+    <row r="90" ht="14.25">
+      <c r="E90" s="7">
         <v>5320</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F90" s="2">
         <v>0.040000000000000001</v>
       </c>
     </row>
-    <row r="81" ht="14.25">
-      <c r="E81">
+    <row r="91" ht="14.25">
+      <c r="E91" s="7">
         <v>5600</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F91" s="2">
         <v>0.040000000000000001</v>
       </c>
     </row>
-    <row r="82" ht="14.25">
-      <c r="E82">
+    <row r="92" ht="14.25">
+      <c r="E92" s="7">
         <v>5840</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F92" s="2">
         <v>0.040000000000000001</v>
       </c>
     </row>
-    <row r="83" ht="14.25">
-      <c r="E83">
+    <row r="93" ht="14.25">
+      <c r="E93" s="7">
         <v>6160</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F93" s="2">
         <v>0.040000000000000001</v>
       </c>
     </row>
-    <row r="84" ht="14.25">
-      <c r="E84">
+    <row r="94" ht="14.25">
+      <c r="E94" s="7">
         <v>6320</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F94" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="85" ht="14.25">
-      <c r="E85">
+    <row r="95" ht="14.25">
+      <c r="E95" s="7">
         <v>6560</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F95" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix errore di battitura
</commit_message>
<xml_diff>
--- a/20240321circuiti2/circuiti_2_dati.xlsx
+++ b/20240321circuiti2/circuiti_2_dati.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RC_vecchio" sheetId="1" state="visible" r:id="rId1"/>
@@ -1961,7 +1961,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2377,7 +2377,7 @@
         <v>640</v>
       </c>
       <c r="F46">
-        <v>250</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" ht="14.25">

</xml_diff>